<commit_message>
Ukończono tworzenie insertów dla obu plików excela zawierających dane z miasta.
</commit_message>
<xml_diff>
--- a/Data/Miasto2.xlsx
+++ b/Data/Miasto2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Zrodla\Harmonogram\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAA7168-F536-425D-85D2-4CF9AD7CBEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7C7128-E429-4CCE-A714-CD92D007EA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2760" windowWidth="29040" windowHeight="15720" tabRatio="419" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t>CHOINKI</t>
   </si>
   <si>
-    <t>ODPADY WIELKOGABARYTOWE</t>
-  </si>
-  <si>
     <t>(http://www.pgk.zamosc.pl/pszok-punkty-selektywnego-zbierania-odpadow-komunalnych-w-zamosciu/)</t>
   </si>
   <si>
@@ -118,27 +115,9 @@
     <t>Zużyta odzież i tekstylia</t>
   </si>
   <si>
-    <t>Zużyty sprzęt elektryczny i elektroniczny</t>
-  </si>
-  <si>
     <t>HARMONOGRAM ODBIORU TWORZYW SZTUCZNYCH I METALU, PAPIERU I TEKTURY, SZKŁA, CHOINEK, ZUŻYTEJ ODZIEŻY, TEKSTYLIÓW,                                                                                            ZUŻYTEGO SPRZETU ELEKTRYCZNEGO I ELEKTRONICZNEGO ORAZ ODPADÓW WIELKOGABARYTOWYCH                                                                                                                                                           W ZABUDOWIE JEDNORODZINNEJ - MIASTO ZAMOŚĆ - 2026r.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Osiedle Koszary, Osiedle Kamienna, Osiedle Planty -  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>zabudowa wielorodzinna</t>
-    </r>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
@@ -173,13 +152,22 @@
   </si>
   <si>
     <t>Rodzaj odpadów</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>MZ108A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -293,13 +281,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="8" tint="-0.249977111117893"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
@@ -596,6 +577,43 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -608,6 +626,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -620,78 +659,20 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1143,8 +1124,8 @@
   </sheetPr>
   <dimension ref="A1:IJ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="80" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A36" zoomScale="115" zoomScaleNormal="80" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,32 +1146,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
+      <c r="A1" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="33"/>
+        <v>34</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="45"/>
       <c r="D2" s="9" t="s">
         <v>12</v>
       </c>
@@ -1229,13 +1210,13 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="25" t="s">
+      <c r="A3" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="25"/>
+      <c r="B3" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="41"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12">
         <v>2</v>
@@ -1264,11 +1245,11 @@
       </c>
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
-      <c r="B4" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="26"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="42"/>
       <c r="D4" s="14">
         <v>5</v>
       </c>
@@ -1295,11 +1276,11 @@
       <c r="O4" s="13"/>
     </row>
     <row r="5" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
-      <c r="B5" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="27"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="43"/>
       <c r="D5" s="14">
         <v>5</v>
       </c>
@@ -1326,11 +1307,11 @@
       <c r="O5" s="13"/>
     </row>
     <row r="6" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
-      <c r="B6" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="28"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="47"/>
       <c r="D6" s="14"/>
       <c r="E6" s="15">
         <v>19</v>
@@ -1349,11 +1330,11 @@
       <c r="O6" s="14"/>
     </row>
     <row r="7" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
-      <c r="B7" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="34"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="25"/>
       <c r="D7" s="14"/>
       <c r="E7" s="15">
         <v>19</v>
@@ -1372,9 +1353,9 @@
       <c r="O7" s="14"/>
     </row>
     <row r="8" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="23"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="14"/>
@@ -1395,11 +1376,11 @@
       <c r="O8" s="14"/>
     </row>
     <row r="9" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="29" t="s">
+      <c r="A9" s="34"/>
+      <c r="B9" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="29"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="14"/>
       <c r="E9" s="15">
         <v>3</v>
@@ -1416,13 +1397,13 @@
       <c r="O9" s="13"/>
     </row>
     <row r="10" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="25"/>
+      <c r="A10" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="41"/>
       <c r="D10" s="12"/>
       <c r="E10" s="18">
         <v>4</v>
@@ -1451,11 +1432,11 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
-      <c r="B11" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="26"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="42"/>
       <c r="D11" s="14">
         <v>7</v>
       </c>
@@ -1482,11 +1463,11 @@
       <c r="O11" s="13"/>
     </row>
     <row r="12" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23"/>
-      <c r="B12" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="27"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="43"/>
       <c r="D12" s="14">
         <v>7</v>
       </c>
@@ -1513,11 +1494,11 @@
       <c r="O12" s="13"/>
     </row>
     <row r="13" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="23"/>
-      <c r="B13" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="35"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="39"/>
       <c r="D13" s="14"/>
       <c r="E13" s="15"/>
       <c r="F13" s="16">
@@ -1536,11 +1517,11 @@
       <c r="O13" s="14"/>
     </row>
     <row r="14" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23"/>
-      <c r="B14" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="34"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="25"/>
       <c r="D14" s="14"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15">
@@ -1559,9 +1540,9 @@
       <c r="O14" s="14"/>
     </row>
     <row r="15" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="23"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="31"/>
       <c r="D15" s="14"/>
@@ -1582,11 +1563,11 @@
       <c r="O15" s="14"/>
     </row>
     <row r="16" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
-      <c r="B16" s="29" t="s">
+      <c r="A16" s="34"/>
+      <c r="B16" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="29"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="14"/>
       <c r="E16" s="15">
         <v>3</v>
@@ -1603,13 +1584,13 @@
       <c r="O16" s="13"/>
     </row>
     <row r="17" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="25"/>
+      <c r="A17" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="41"/>
       <c r="D17" s="12"/>
       <c r="E17" s="18">
         <v>6</v>
@@ -1638,11 +1619,11 @@
       </c>
     </row>
     <row r="18" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="23"/>
-      <c r="B18" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="42"/>
       <c r="D18" s="14">
         <v>8</v>
       </c>
@@ -1669,11 +1650,11 @@
       <c r="O18" s="13"/>
     </row>
     <row r="19" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="23"/>
-      <c r="B19" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="27"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="43"/>
       <c r="D19" s="14">
         <v>8</v>
       </c>
@@ -1700,11 +1681,11 @@
       <c r="O19" s="13"/>
     </row>
     <row r="20" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="23"/>
-      <c r="B20" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="35"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="39"/>
       <c r="D20" s="14"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15">
@@ -1723,11 +1704,11 @@
       <c r="O20" s="14"/>
     </row>
     <row r="21" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="23"/>
-      <c r="B21" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="34"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="25"/>
       <c r="D21" s="14"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15">
@@ -1746,9 +1727,9 @@
       <c r="O21" s="14"/>
     </row>
     <row r="22" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="23"/>
+      <c r="A22" s="33"/>
       <c r="B22" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="31"/>
       <c r="D22" s="14"/>
@@ -1769,11 +1750,11 @@
       <c r="O22" s="14"/>
     </row>
     <row r="23" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="24"/>
-      <c r="B23" s="29" t="s">
+      <c r="A23" s="34"/>
+      <c r="B23" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="29"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="14"/>
       <c r="E23" s="15">
         <v>2</v>
@@ -1790,13 +1771,13 @@
       <c r="O23" s="13"/>
     </row>
     <row r="24" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="25"/>
+      <c r="A24" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="41"/>
       <c r="D24" s="12"/>
       <c r="E24" s="18">
         <v>25</v>
@@ -1825,11 +1806,11 @@
       </c>
     </row>
     <row r="25" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="23"/>
-      <c r="B25" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="26"/>
+      <c r="A25" s="33"/>
+      <c r="B25" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="42"/>
       <c r="D25" s="14">
         <v>13</v>
       </c>
@@ -1856,11 +1837,11 @@
       <c r="O25" s="13"/>
     </row>
     <row r="26" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="23"/>
-      <c r="B26" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="27"/>
+      <c r="A26" s="33"/>
+      <c r="B26" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="43"/>
       <c r="D26" s="14">
         <v>13</v>
       </c>
@@ -1887,11 +1868,11 @@
       <c r="O26" s="13"/>
     </row>
     <row r="27" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="23"/>
-      <c r="B27" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="35"/>
+      <c r="A27" s="33"/>
+      <c r="B27" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="39"/>
       <c r="D27" s="14"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15">
@@ -1910,11 +1891,11 @@
       <c r="O27" s="14"/>
     </row>
     <row r="28" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="23"/>
-      <c r="B28" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="34"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="25"/>
       <c r="D28" s="14"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15">
@@ -1933,9 +1914,9 @@
       <c r="O28" s="14"/>
     </row>
     <row r="29" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="23"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="31"/>
       <c r="D29" s="14"/>
@@ -1956,11 +1937,11 @@
       <c r="O29" s="14"/>
     </row>
     <row r="30" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="24"/>
-      <c r="B30" s="29" t="s">
+      <c r="A30" s="34"/>
+      <c r="B30" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="29"/>
+      <c r="C30" s="44"/>
       <c r="D30" s="14"/>
       <c r="E30" s="15">
         <v>6</v>
@@ -1977,13 +1958,13 @@
       <c r="O30" s="13"/>
     </row>
     <row r="31" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="25"/>
+      <c r="A31" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="41"/>
       <c r="D31" s="12"/>
       <c r="E31" s="18">
         <v>25</v>
@@ -2012,11 +1993,11 @@
       </c>
     </row>
     <row r="32" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="23"/>
-      <c r="B32" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="26"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="42"/>
       <c r="D32" s="14">
         <v>13</v>
       </c>
@@ -2043,11 +2024,11 @@
       <c r="O32" s="13"/>
     </row>
     <row r="33" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="23"/>
-      <c r="B33" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="27"/>
+      <c r="A33" s="33"/>
+      <c r="B33" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="43"/>
       <c r="D33" s="14">
         <v>13</v>
       </c>
@@ -2074,11 +2055,11 @@
       <c r="O33" s="13"/>
     </row>
     <row r="34" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="23"/>
-      <c r="B34" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="35"/>
+      <c r="A34" s="33"/>
+      <c r="B34" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="39"/>
       <c r="D34" s="14"/>
       <c r="E34" s="15"/>
       <c r="F34" s="15">
@@ -2097,11 +2078,11 @@
       <c r="O34" s="14"/>
     </row>
     <row r="35" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="23"/>
-      <c r="B35" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="34"/>
+      <c r="A35" s="33"/>
+      <c r="B35" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="25"/>
       <c r="D35" s="14"/>
       <c r="E35" s="15"/>
       <c r="F35" s="15">
@@ -2120,9 +2101,9 @@
       <c r="O35" s="14"/>
     </row>
     <row r="36" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="23"/>
+      <c r="A36" s="33"/>
       <c r="B36" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" s="31"/>
       <c r="D36" s="14"/>
@@ -2143,11 +2124,11 @@
       <c r="O36" s="14"/>
     </row>
     <row r="37" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="24"/>
-      <c r="B37" s="29" t="s">
+      <c r="A37" s="34"/>
+      <c r="B37" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="29"/>
+      <c r="C37" s="44"/>
       <c r="D37" s="14"/>
       <c r="E37" s="15">
         <v>6</v>
@@ -2164,13 +2145,13 @@
       <c r="O37" s="13"/>
     </row>
     <row r="38" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C38" s="25"/>
+      <c r="A38" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="41"/>
       <c r="D38" s="12"/>
       <c r="E38" s="18">
         <v>25</v>
@@ -2199,11 +2180,11 @@
       </c>
     </row>
     <row r="39" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="23"/>
-      <c r="B39" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" s="26"/>
+      <c r="A39" s="33"/>
+      <c r="B39" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="42"/>
       <c r="D39" s="14">
         <v>21</v>
       </c>
@@ -2230,11 +2211,11 @@
       <c r="O39" s="13"/>
     </row>
     <row r="40" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="23"/>
-      <c r="B40" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="27"/>
+      <c r="A40" s="33"/>
+      <c r="B40" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="43"/>
       <c r="D40" s="14">
         <v>21</v>
       </c>
@@ -2261,11 +2242,11 @@
       <c r="O40" s="13"/>
     </row>
     <row r="41" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="23"/>
-      <c r="B41" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="35"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="39"/>
       <c r="D41" s="14"/>
       <c r="E41" s="15"/>
       <c r="F41" s="15"/>
@@ -2284,11 +2265,11 @@
       <c r="O41" s="14"/>
     </row>
     <row r="42" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="23"/>
-      <c r="B42" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" s="34"/>
+      <c r="A42" s="33"/>
+      <c r="B42" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="25"/>
       <c r="D42" s="14"/>
       <c r="E42" s="15"/>
       <c r="F42" s="15"/>
@@ -2307,9 +2288,9 @@
       <c r="O42" s="14"/>
     </row>
     <row r="43" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="23"/>
+      <c r="A43" s="33"/>
       <c r="B43" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C43" s="31"/>
       <c r="D43" s="14"/>
@@ -2330,11 +2311,11 @@
       <c r="O43" s="14"/>
     </row>
     <row r="44" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="24"/>
-      <c r="B44" s="29" t="s">
+      <c r="A44" s="34"/>
+      <c r="B44" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="29"/>
+      <c r="C44" s="44"/>
       <c r="D44" s="14"/>
       <c r="E44" s="15">
         <v>4</v>
@@ -2351,13 +2332,13 @@
       <c r="O44" s="13"/>
     </row>
     <row r="45" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B45" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C45" s="25"/>
+      <c r="A45" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="41"/>
       <c r="D45" s="12"/>
       <c r="E45" s="18">
         <v>25</v>
@@ -2386,11 +2367,11 @@
       </c>
     </row>
     <row r="46" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="36"/>
-      <c r="B46" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C46" s="26"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="42"/>
       <c r="D46" s="14">
         <v>21</v>
       </c>
@@ -2417,11 +2398,11 @@
       <c r="O46" s="13"/>
     </row>
     <row r="47" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="36"/>
-      <c r="B47" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" s="27"/>
+      <c r="A47" s="40"/>
+      <c r="B47" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="43"/>
       <c r="D47" s="14">
         <v>21</v>
       </c>
@@ -2448,11 +2429,11 @@
       <c r="O47" s="13"/>
     </row>
     <row r="48" spans="1:15" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="36"/>
-      <c r="B48" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C48" s="35"/>
+      <c r="A48" s="40"/>
+      <c r="B48" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="39"/>
       <c r="D48" s="14"/>
       <c r="E48" s="15"/>
       <c r="F48" s="15"/>
@@ -2471,11 +2452,11 @@
       <c r="O48" s="14"/>
     </row>
     <row r="49" spans="1:244" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="36"/>
-      <c r="B49" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C49" s="34"/>
+      <c r="A49" s="40"/>
+      <c r="B49" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="25"/>
       <c r="D49" s="14"/>
       <c r="E49" s="15"/>
       <c r="F49" s="15"/>
@@ -2494,9 +2475,9 @@
       <c r="O49" s="14"/>
     </row>
     <row r="50" spans="1:244" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="36"/>
+      <c r="A50" s="40"/>
       <c r="B50" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C50" s="31"/>
       <c r="D50" s="14"/>
@@ -2517,11 +2498,11 @@
       <c r="O50" s="14"/>
     </row>
     <row r="51" spans="1:244" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="36"/>
-      <c r="B51" s="29" t="s">
+      <c r="A51" s="40"/>
+      <c r="B51" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C51" s="29"/>
+      <c r="C51" s="44"/>
       <c r="D51" s="13"/>
       <c r="E51" s="17">
         <v>4</v>
@@ -2538,13 +2519,13 @@
       <c r="O51" s="13"/>
     </row>
     <row r="52" spans="1:244" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="C52" s="47"/>
+      <c r="A52" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52" s="36"/>
       <c r="D52" s="14"/>
       <c r="E52" s="15"/>
       <c r="F52" s="15">
@@ -2563,11 +2544,11 @@
       <c r="O52" s="14"/>
     </row>
     <row r="53" spans="1:244" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="23"/>
-      <c r="B53" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53" s="34"/>
+      <c r="A53" s="33"/>
+      <c r="B53" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" s="25"/>
       <c r="D53" s="14"/>
       <c r="E53" s="15"/>
       <c r="F53" s="15">
@@ -2586,9 +2567,9 @@
       <c r="O53" s="14"/>
     </row>
     <row r="54" spans="1:244" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="23"/>
+      <c r="A54" s="33"/>
       <c r="B54" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C54" s="31"/>
       <c r="D54" s="20"/>
@@ -2609,11 +2590,11 @@
       <c r="O54" s="20"/>
     </row>
     <row r="55" spans="1:244" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="24"/>
-      <c r="B55" s="42" t="s">
+      <c r="A55" s="34"/>
+      <c r="B55" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="43"/>
+      <c r="C55" s="27"/>
       <c r="D55" s="13"/>
       <c r="E55" s="17">
         <v>2</v>
@@ -2630,46 +2611,46 @@
       <c r="O55" s="13"/>
     </row>
     <row r="56" spans="1:244" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="B56" s="44"/>
-      <c r="C56" s="44"/>
-      <c r="D56" s="44"/>
-      <c r="E56" s="44"/>
-      <c r="F56" s="44"/>
-      <c r="G56" s="44"/>
-      <c r="H56" s="44"/>
-      <c r="I56" s="44"/>
-      <c r="J56" s="44"/>
-      <c r="K56" s="44"/>
-      <c r="L56" s="44"/>
-      <c r="M56" s="44"/>
-      <c r="N56" s="44"/>
-      <c r="O56" s="44"/>
+      <c r="A56" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="28"/>
+      <c r="I56" s="28"/>
+      <c r="J56" s="28"/>
+      <c r="K56" s="28"/>
+      <c r="L56" s="28"/>
+      <c r="M56" s="28"/>
+      <c r="N56" s="28"/>
+      <c r="O56" s="28"/>
     </row>
     <row r="57" spans="1:244" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="45"/>
-      <c r="C57" s="45"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="45"/>
-      <c r="F57" s="45"/>
-      <c r="G57" s="45"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="45"/>
-      <c r="J57" s="45"/>
-      <c r="K57" s="45"/>
-      <c r="L57" s="45"/>
-      <c r="M57" s="45"/>
-      <c r="N57" s="45"/>
-      <c r="O57" s="45"/>
+      <c r="A57" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" s="29"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="29"/>
+      <c r="H57" s="29"/>
+      <c r="I57" s="29"/>
+      <c r="J57" s="29"/>
+      <c r="K57" s="29"/>
+      <c r="L57" s="29"/>
+      <c r="M57" s="29"/>
+      <c r="N57" s="29"/>
+      <c r="O57" s="29"/>
     </row>
     <row r="58" spans="1:244" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B58" s="37"/>
       <c r="C58" s="37"/>
@@ -2688,7 +2669,7 @@
     </row>
     <row r="59" spans="1:244" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B59" s="38"/>
       <c r="C59" s="38"/>
@@ -2706,23 +2687,23 @@
       <c r="O59" s="38"/>
     </row>
     <row r="60" spans="1:244" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="39" t="s">
+      <c r="A60" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B60" s="39"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="39"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="39"/>
-      <c r="I60" s="39"/>
-      <c r="J60" s="39"/>
-      <c r="K60" s="39"/>
-      <c r="L60" s="39"/>
-      <c r="M60" s="39"/>
-      <c r="N60" s="39"/>
-      <c r="O60" s="39"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="22"/>
+      <c r="J60" s="22"/>
+      <c r="K60" s="22"/>
+      <c r="L60" s="22"/>
+      <c r="M60" s="22"/>
+      <c r="N60" s="22"/>
+      <c r="O60" s="22"/>
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
@@ -2954,23 +2935,23 @@
       <c r="IJ60" s="2"/>
     </row>
     <row r="61" spans="1:244" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="B61" s="39"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="39"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="39"/>
-      <c r="I61" s="39"/>
-      <c r="J61" s="39"/>
-      <c r="K61" s="39"/>
-      <c r="L61" s="39"/>
-      <c r="M61" s="39"/>
-      <c r="N61" s="39"/>
-      <c r="O61" s="39"/>
+      <c r="A61" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="22"/>
+      <c r="I61" s="22"/>
+      <c r="J61" s="22"/>
+      <c r="K61" s="22"/>
+      <c r="L61" s="22"/>
+      <c r="M61" s="22"/>
+      <c r="N61" s="22"/>
+      <c r="O61" s="22"/>
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
@@ -3202,60 +3183,85 @@
       <c r="IJ61" s="2"/>
     </row>
     <row r="62" spans="1:244" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="40" t="s">
+      <c r="A62" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B62" s="40"/>
-      <c r="C62" s="40"/>
-      <c r="D62" s="40"/>
-      <c r="E62" s="40"/>
-      <c r="F62" s="40"/>
-      <c r="G62" s="40"/>
-      <c r="H62" s="40"/>
-      <c r="I62" s="40"/>
-      <c r="J62" s="40"/>
-      <c r="K62" s="40"/>
-      <c r="L62" s="40"/>
-      <c r="M62" s="40"/>
-      <c r="N62" s="40"/>
-      <c r="O62" s="40"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="23"/>
+      <c r="H62" s="23"/>
+      <c r="I62" s="23"/>
+      <c r="J62" s="23"/>
+      <c r="K62" s="23"/>
+      <c r="L62" s="23"/>
+      <c r="M62" s="23"/>
+      <c r="N62" s="23"/>
+      <c r="O62" s="23"/>
     </row>
     <row r="63" spans="1:244" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="41" t="s">
+      <c r="A63" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B63" s="41"/>
-      <c r="C63" s="41"/>
-      <c r="D63" s="41"/>
-      <c r="E63" s="41"/>
-      <c r="F63" s="41"/>
-      <c r="G63" s="41"/>
-      <c r="H63" s="41"/>
-      <c r="I63" s="41"/>
-      <c r="J63" s="41"/>
-      <c r="K63" s="41"/>
-      <c r="L63" s="41"/>
-      <c r="M63" s="41"/>
-      <c r="N63" s="41"/>
-      <c r="O63" s="41"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="24"/>
+      <c r="H63" s="24"/>
+      <c r="I63" s="24"/>
+      <c r="J63" s="24"/>
+      <c r="K63" s="24"/>
+      <c r="L63" s="24"/>
+      <c r="M63" s="24"/>
+      <c r="N63" s="24"/>
+      <c r="O63" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="A61:O61"/>
-    <mergeCell ref="A62:O62"/>
-    <mergeCell ref="A63:O63"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="A56:O56"/>
-    <mergeCell ref="A57:O57"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="A52:A55"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="A58:O58"/>
-    <mergeCell ref="A59:O59"/>
-    <mergeCell ref="A60:O60"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="A31:A37"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B30:C30"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="B42:C42"/>
@@ -3272,46 +3278,21 @@
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="A31:A37"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="A58:O58"/>
+    <mergeCell ref="A59:O59"/>
+    <mergeCell ref="A60:O60"/>
+    <mergeCell ref="A61:O61"/>
+    <mergeCell ref="A62:O62"/>
+    <mergeCell ref="A63:O63"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="A56:O56"/>
+    <mergeCell ref="A57:O57"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="B52:C52"/>
   </mergeCells>
   <pageMargins left="0.19184027777777779" right="0.15748031496062992" top="0.16866319444444444" bottom="0.15748031496062992" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="69" firstPageNumber="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>